<commit_message>
adicionando a la lista 2 mas
</commit_message>
<xml_diff>
--- a/storage/excel/imports/Casos de Amortización de Deuda.xlsx
+++ b/storage/excel/imports/Casos de Amortización de Deuda.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="12915"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="27870" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="5" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$F$1:$F$26</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="104">
   <si>
     <t xml:space="preserve">PEREZ               </t>
   </si>
@@ -327,6 +330,15 @@
   </si>
   <si>
     <t>3,705.61</t>
+  </si>
+  <si>
+    <t>GALLARDO</t>
+  </si>
+  <si>
+    <t>VACAFLOR</t>
+  </si>
+  <si>
+    <t>CRISOSTOMO</t>
   </si>
 </sst>
 </file>
@@ -964,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD32"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2004,7 +2016,63 @@
         <v>100</v>
       </c>
     </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>3956</v>
+      </c>
+      <c r="C27">
+        <v>1665214</v>
+      </c>
+      <c r="D27" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" t="s">
+        <v>103</v>
+      </c>
+      <c r="J27" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="K27">
+        <v>7431.04</v>
+      </c>
+      <c r="L27">
+        <v>4696.5600000000004</v>
+      </c>
+      <c r="M27" s="37">
+        <v>2734.48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>3955</v>
+      </c>
+      <c r="C28">
+        <v>2323723</v>
+      </c>
+      <c r="J28" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="K28">
+        <v>7503.18</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28" s="37">
+        <v>7503.18</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="F1:F26"/>
   <pageMargins left="0.19685039370078741" right="0.15748031496062992" top="0.35433070866141736" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="90" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>